<commit_message>
Tried first alternate. Same as mine, different order
</commit_message>
<xml_diff>
--- a/CH-151 Solid Worl.xlsx
+++ b/CH-151 Solid Worl.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95297C4-D9FC-4770-BD73-AB76D95F3CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC66700-A679-4279-B18A-44E16D70AF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="MySingle" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt1'!$B$2:$G$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$G$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingle!$B$2:$G$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$G$14</definedName>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
@@ -110,6 +112,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
+  </si>
+  <si>
+    <t>This solution is similar to mine, just did operations in different order.</t>
   </si>
 </sst>
 </file>
@@ -2028,7 +2033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961BE012-33E9-45FA-8E02-97B21AB8D3FF}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -2659,4 +2664,437 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B2617D-69A9-4F41-984A-874633BD787D}">
+  <dimension ref="A1:P20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="6" width="10.59765625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="8" max="8" width="8.69921875" style="5" customWidth="1"/>
+    <col min="9" max="10" width="8.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="H1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="M1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="20">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21">
+        <v>-8.1120029900000006</v>
+      </c>
+      <c r="D3" s="21">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="E3" s="22">
+        <v>2</v>
+      </c>
+      <c r="F3" s="23">
+        <v>-12.714630403999999</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="39">
+        <v>1</v>
+      </c>
+      <c r="I3" s="40">
+        <v>-8.1120029900000006</v>
+      </c>
+      <c r="J3" s="41">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="C4" s="25">
+        <v>3</v>
+      </c>
+      <c r="D4" s="25">
+        <v>-10.905970308000001</v>
+      </c>
+      <c r="E4" s="25">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="F4" s="26"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="42">
+        <v>2</v>
+      </c>
+      <c r="I4" s="43">
+        <v>-12.714630403999999</v>
+      </c>
+      <c r="J4" s="44">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="27">
+        <v>4</v>
+      </c>
+      <c r="C5" s="28">
+        <v>-6.9681729509999997</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="45">
+        <v>3</v>
+      </c>
+      <c r="I5" s="46">
+        <v>-10.905970308000001</v>
+      </c>
+      <c r="J5" s="47">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="28">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="D6" s="31">
+        <v>5</v>
+      </c>
+      <c r="E6" s="31">
+        <v>9.8603081269999997</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="48">
+        <v>4</v>
+      </c>
+      <c r="I6" s="49">
+        <v>-6.9681729509999997</v>
+      </c>
+      <c r="J6" s="50">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="32">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="C7" s="33">
+        <v>6</v>
+      </c>
+      <c r="D7" s="33">
+        <v>15.281757216999999</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="51">
+        <v>5</v>
+      </c>
+      <c r="I7" s="52">
+        <v>9.8603081269999997</v>
+      </c>
+      <c r="J7" s="53">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="33">
+        <v>15.480173389000001</v>
+      </c>
+      <c r="D8" s="34">
+        <v>7</v>
+      </c>
+      <c r="E8" s="34">
+        <v>-1.6866469639999999</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="15">
+        <v>6</v>
+      </c>
+      <c r="I8" s="16">
+        <v>15.281757216999999</v>
+      </c>
+      <c r="J8" s="17">
+        <v>15.480173389000001</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="35">
+        <v>14.238796785</v>
+      </c>
+      <c r="C9" s="29">
+        <v>8</v>
+      </c>
+      <c r="D9" s="29">
+        <v>5.5603806660000004</v>
+      </c>
+      <c r="E9" s="29">
+        <v>7.5524191150000002</v>
+      </c>
+      <c r="F9" s="26">
+        <v>9</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="15">
+        <v>7</v>
+      </c>
+      <c r="I9" s="54">
+        <v>-1.6866469639999999</v>
+      </c>
+      <c r="J9" s="18">
+        <v>14.238796785</v>
+      </c>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="36">
+        <v>13.491118387</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="37">
+        <v>11.082843070999999</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="55">
+        <v>8</v>
+      </c>
+      <c r="I10" s="54">
+        <v>5.5603806660000004</v>
+      </c>
+      <c r="J10" s="18">
+        <v>7.5524191150000002</v>
+      </c>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="56">
+        <v>9</v>
+      </c>
+      <c r="I11" s="19">
+        <v>13.491118387</v>
+      </c>
+      <c r="J11" s="57">
+        <v>11.082843070999999</v>
+      </c>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" cm="1">
+        <f t="array" ref="C12:E20">_xlfn.LET(
+_xlpm.d, B3:F10,
+_xlpm.df, IF((ISTEXT(_xlpm.d))+(_xlpm.d=0),NA(),_xlpm.d),
+_xlfn.WRAPROWS(_xlfn.TOCOL(_xlpm.df,3),3)
+)</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>-8.1120029900000006</v>
+      </c>
+      <c r="E12" s="7">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7">
+        <v>-12.714630403999999</v>
+      </c>
+      <c r="E13" s="7">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7">
+        <v>3</v>
+      </c>
+      <c r="D14" s="7">
+        <v>-10.905970308000001</v>
+      </c>
+      <c r="E14" s="7">
+        <v>49.496281891999999</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="7">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>-6.9681729509999997</v>
+      </c>
+      <c r="E15" s="7">
+        <v>49.496281891999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>9.8603081269999997</v>
+      </c>
+      <c r="E16" s="4">
+        <v>49.496281891999999</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="4">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4">
+        <v>15.281757216999999</v>
+      </c>
+      <c r="E17" s="4">
+        <v>15.480173389000001</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="4">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-1.6866469639999999</v>
+      </c>
+      <c r="E18" s="4">
+        <v>14.238796785</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="4">
+        <v>8</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5.5603806660000004</v>
+      </c>
+      <c r="E19" s="4">
+        <v>7.5524191150000002</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="4">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4">
+        <v>13.491118387</v>
+      </c>
+      <c r="E20" s="4">
+        <v>11.082843070999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>